<commit_message>
added number-of-remissions extension to condition profile
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-msdiagnosis.xlsx
+++ b/docs/StructureDefinition-msdiagnosis.xlsx
@@ -10,13 +10,13 @@
     <sheet name="Elements" r:id="rId4" sheetId="2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AO$66</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AO$67</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2473" uniqueCount="455">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2508" uniqueCount="460">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-07-26T16:47:03-05:00</t>
+    <t>2022-07-28T10:15:20-05:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -732,10 +732,27 @@
     <t>Condition.extension</t>
   </si>
   <si>
-    <t>May be used to represent additional information that is not part of the basic definition of the resource. To make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
+    <t>Extension</t>
+  </si>
+  <si>
+    <t>An Extension</t>
   </si>
   <si>
     <t>DomainResource.extension</t>
+  </si>
+  <si>
+    <t>NumberOfRemissions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {http://fhir.nmdp.org/ig/matchsource/StructureDefinition/number-of-remissions}
+</t>
+  </si>
+  <si>
+    <t>Number of Remissions of Primary Diagnosis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ele-1
+</t>
   </si>
   <si>
     <t>Condition.modifierExtension</t>
@@ -1746,7 +1763,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AO66"/>
+  <dimension ref="A1:AO67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1756,7 +1773,7 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="42.5390625" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="18.5859375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="20.47265625" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="5.8984375" customWidth="true" bestFit="true" hidden="true"/>
     <col min="5" max="5" width="4.69921875" customWidth="true" bestFit="true"/>
@@ -4618,7 +4635,7 @@
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" t="s" s="2">
@@ -4640,14 +4657,12 @@
         <v>106</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>107</v>
+        <v>231</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>231</v>
-      </c>
-      <c r="M25" t="s" s="2">
-        <v>109</v>
-      </c>
+        <v>232</v>
+      </c>
+      <c r="M25" s="2"/>
       <c r="N25" s="2"/>
       <c r="O25" t="s" s="2">
         <v>75</v>
@@ -4684,19 +4699,17 @@
         <v>75</v>
       </c>
       <c r="AA25" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AB25" t="s" s="2">
-        <v>75</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="AB25" s="2"/>
       <c r="AC25" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AD25" t="s" s="2">
-        <v>75</v>
+        <v>112</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>76</v>
@@ -4720,7 +4733,7 @@
         <v>75</v>
       </c>
       <c r="AM25" t="s" s="2">
-        <v>229</v>
+        <v>75</v>
       </c>
       <c r="AN25" t="s" s="2">
         <v>75</v>
@@ -4731,43 +4744,41 @@
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>233</v>
-      </c>
-      <c r="B26" s="2"/>
+        <v>230</v>
+      </c>
+      <c r="B26" t="s" s="2">
+        <v>234</v>
+      </c>
       <c r="C26" t="s" s="2">
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" t="s" s="2">
         <v>76</v>
       </c>
       <c r="F26" t="s" s="2">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="G26" t="s" s="2">
         <v>75</v>
       </c>
       <c r="H26" t="s" s="2">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="I26" t="s" s="2">
         <v>75</v>
       </c>
       <c r="J26" t="s" s="2">
-        <v>106</v>
+        <v>235</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>235</v>
-      </c>
-      <c r="M26" t="s" s="2">
-        <v>109</v>
-      </c>
-      <c r="N26" t="s" s="2">
         <v>236</v>
       </c>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
       <c r="O26" t="s" s="2">
         <v>75</v>
       </c>
@@ -4815,7 +4826,7 @@
         <v>75</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>76</v>
@@ -4824,7 +4835,7 @@
         <v>77</v>
       </c>
       <c r="AH26" t="s" s="2">
-        <v>75</v>
+        <v>237</v>
       </c>
       <c r="AI26" t="s" s="2">
         <v>114</v>
@@ -4839,7 +4850,7 @@
         <v>75</v>
       </c>
       <c r="AM26" t="s" s="2">
-        <v>229</v>
+        <v>75</v>
       </c>
       <c r="AN26" t="s" s="2">
         <v>75</v>
@@ -4854,7 +4865,7 @@
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
-        <v>75</v>
+        <v>105</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" t="s" s="2">
@@ -4867,25 +4878,25 @@
         <v>75</v>
       </c>
       <c r="H27" t="s" s="2">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="I27" t="s" s="2">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="J27" t="s" s="2">
+        <v>106</v>
+      </c>
+      <c r="K27" t="s" s="2">
         <v>239</v>
       </c>
-      <c r="K27" t="s" s="2">
+      <c r="L27" t="s" s="2">
         <v>240</v>
       </c>
-      <c r="L27" t="s" s="2">
+      <c r="M27" t="s" s="2">
+        <v>109</v>
+      </c>
+      <c r="N27" t="s" s="2">
         <v>241</v>
-      </c>
-      <c r="M27" t="s" s="2">
-        <v>242</v>
-      </c>
-      <c r="N27" t="s" s="2">
-        <v>243</v>
       </c>
       <c r="O27" t="s" s="2">
         <v>75</v>
@@ -4934,7 +4945,7 @@
         <v>75</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>76</v>
@@ -4946,10 +4957,10 @@
         <v>75</v>
       </c>
       <c r="AI27" t="s" s="2">
-        <v>98</v>
+        <v>114</v>
       </c>
       <c r="AJ27" t="s" s="2">
-        <v>244</v>
+        <v>75</v>
       </c>
       <c r="AK27" t="s" s="2">
         <v>75</v>
@@ -4958,10 +4969,10 @@
         <v>75</v>
       </c>
       <c r="AM27" t="s" s="2">
-        <v>245</v>
+        <v>229</v>
       </c>
       <c r="AN27" t="s" s="2">
-        <v>246</v>
+        <v>75</v>
       </c>
       <c r="AO27" t="s" s="2">
         <v>75</v>
@@ -4969,7 +4980,7 @@
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -4980,30 +4991,32 @@
         <v>76</v>
       </c>
       <c r="F28" t="s" s="2">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="G28" t="s" s="2">
         <v>75</v>
       </c>
       <c r="H28" t="s" s="2">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="I28" t="s" s="2">
         <v>87</v>
       </c>
       <c r="J28" t="s" s="2">
+        <v>244</v>
+      </c>
+      <c r="K28" t="s" s="2">
+        <v>245</v>
+      </c>
+      <c r="L28" t="s" s="2">
+        <v>246</v>
+      </c>
+      <c r="M28" t="s" s="2">
+        <v>247</v>
+      </c>
+      <c r="N28" t="s" s="2">
         <v>248</v>
       </c>
-      <c r="K28" t="s" s="2">
-        <v>249</v>
-      </c>
-      <c r="L28" t="s" s="2">
-        <v>250</v>
-      </c>
-      <c r="M28" t="s" s="2">
-        <v>251</v>
-      </c>
-      <c r="N28" s="2"/>
       <c r="O28" t="s" s="2">
         <v>75</v>
       </c>
@@ -5027,13 +5040,13 @@
         <v>75</v>
       </c>
       <c r="W28" t="s" s="2">
-        <v>252</v>
+        <v>75</v>
       </c>
       <c r="X28" t="s" s="2">
-        <v>253</v>
+        <v>75</v>
       </c>
       <c r="Y28" t="s" s="2">
-        <v>254</v>
+        <v>75</v>
       </c>
       <c r="Z28" t="s" s="2">
         <v>75</v>
@@ -5051,34 +5064,34 @@
         <v>75</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AG28" t="s" s="2">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="AH28" t="s" s="2">
-        <v>255</v>
+        <v>75</v>
       </c>
       <c r="AI28" t="s" s="2">
         <v>98</v>
       </c>
       <c r="AJ28" t="s" s="2">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="AK28" t="s" s="2">
-        <v>257</v>
+        <v>75</v>
       </c>
       <c r="AL28" t="s" s="2">
-        <v>258</v>
+        <v>75</v>
       </c>
       <c r="AM28" t="s" s="2">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="AN28" t="s" s="2">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="AO28" t="s" s="2">
         <v>75</v>
@@ -5086,7 +5099,7 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -5109,16 +5122,16 @@
         <v>87</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="N29" s="2"/>
       <c r="O29" t="s" s="2">
@@ -5144,31 +5157,31 @@
         <v>75</v>
       </c>
       <c r="W29" t="s" s="2">
+        <v>257</v>
+      </c>
+      <c r="X29" t="s" s="2">
+        <v>258</v>
+      </c>
+      <c r="Y29" t="s" s="2">
+        <v>259</v>
+      </c>
+      <c r="Z29" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AA29" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AB29" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AC29" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AD29" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AE29" t="s" s="2">
         <v>252</v>
-      </c>
-      <c r="X29" t="s" s="2">
-        <v>265</v>
-      </c>
-      <c r="Y29" t="s" s="2">
-        <v>266</v>
-      </c>
-      <c r="Z29" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AA29" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AB29" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AC29" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AD29" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AE29" t="s" s="2">
-        <v>261</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>76</v>
@@ -5177,33 +5190,33 @@
         <v>86</v>
       </c>
       <c r="AH29" t="s" s="2">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="AI29" t="s" s="2">
         <v>98</v>
       </c>
       <c r="AJ29" t="s" s="2">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="AK29" t="s" s="2">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="AL29" t="s" s="2">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="AM29" t="s" s="2">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="AN29" t="s" s="2">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="AO29" t="s" s="2">
-        <v>271</v>
+        <v>75</v>
       </c>
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -5214,28 +5227,28 @@
         <v>76</v>
       </c>
       <c r="F30" t="s" s="2">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="G30" t="s" s="2">
         <v>75</v>
       </c>
       <c r="H30" t="s" s="2">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="I30" t="s" s="2">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="N30" s="2"/>
       <c r="O30" t="s" s="2">
@@ -5261,13 +5274,13 @@
         <v>75</v>
       </c>
       <c r="W30" t="s" s="2">
-        <v>144</v>
+        <v>257</v>
       </c>
       <c r="X30" t="s" s="2">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="Y30" t="s" s="2">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="Z30" t="s" s="2">
         <v>75</v>
@@ -5285,42 +5298,42 @@
         <v>75</v>
       </c>
       <c r="AE30" t="s" s="2">
+        <v>266</v>
+      </c>
+      <c r="AF30" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AG30" t="s" s="2">
+        <v>86</v>
+      </c>
+      <c r="AH30" t="s" s="2">
         <v>272</v>
-      </c>
-      <c r="AF30" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AG30" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AH30" t="s" s="2">
-        <v>75</v>
       </c>
       <c r="AI30" t="s" s="2">
         <v>98</v>
       </c>
       <c r="AJ30" t="s" s="2">
-        <v>75</v>
+        <v>261</v>
       </c>
       <c r="AK30" t="s" s="2">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="AL30" t="s" s="2">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="AM30" t="s" s="2">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="AN30" t="s" s="2">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="AO30" t="s" s="2">
-        <v>75</v>
+        <v>276</v>
       </c>
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -5331,7 +5344,7 @@
         <v>76</v>
       </c>
       <c r="F31" t="s" s="2">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="G31" t="s" s="2">
         <v>75</v>
@@ -5343,16 +5356,16 @@
         <v>75</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="N31" s="2"/>
       <c r="O31" t="s" s="2">
@@ -5378,13 +5391,13 @@
         <v>75</v>
       </c>
       <c r="W31" t="s" s="2">
-        <v>210</v>
+        <v>144</v>
       </c>
       <c r="X31" t="s" s="2">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="Y31" t="s" s="2">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="Z31" t="s" s="2">
         <v>75</v>
@@ -5402,13 +5415,13 @@
         <v>75</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AG31" t="s" s="2">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="AH31" t="s" s="2">
         <v>75</v>
@@ -5420,58 +5433,58 @@
         <v>75</v>
       </c>
       <c r="AK31" t="s" s="2">
+        <v>282</v>
+      </c>
+      <c r="AL31" t="s" s="2">
+        <v>283</v>
+      </c>
+      <c r="AM31" t="s" s="2">
+        <v>284</v>
+      </c>
+      <c r="AN31" t="s" s="2">
+        <v>285</v>
+      </c>
+      <c r="AO31" t="s" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="32" hidden="true">
+      <c r="A32" t="s" s="2">
         <v>286</v>
-      </c>
-      <c r="AL31" t="s" s="2">
-        <v>287</v>
-      </c>
-      <c r="AM31" t="s" s="2">
-        <v>288</v>
-      </c>
-      <c r="AN31" t="s" s="2">
-        <v>289</v>
-      </c>
-      <c r="AO31" t="s" s="2">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="s" s="2">
-        <v>291</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
-        <v>292</v>
+        <v>75</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" t="s" s="2">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="F32" t="s" s="2">
         <v>86</v>
       </c>
       <c r="G32" t="s" s="2">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="H32" t="s" s="2">
         <v>75</v>
       </c>
       <c r="I32" t="s" s="2">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="J32" t="s" s="2">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>294</v>
-      </c>
-      <c r="M32" s="2"/>
-      <c r="N32" t="s" s="2">
-        <v>295</v>
-      </c>
+        <v>288</v>
+      </c>
+      <c r="M32" t="s" s="2">
+        <v>289</v>
+      </c>
+      <c r="N32" s="2"/>
       <c r="O32" t="s" s="2">
         <v>75</v>
       </c>
@@ -5495,11 +5508,13 @@
         <v>75</v>
       </c>
       <c r="W32" t="s" s="2">
-        <v>252</v>
-      </c>
-      <c r="X32" s="2"/>
+        <v>210</v>
+      </c>
+      <c r="X32" t="s" s="2">
+        <v>288</v>
+      </c>
       <c r="Y32" t="s" s="2">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="Z32" t="s" s="2">
         <v>75</v>
@@ -5517,7 +5532,7 @@
         <v>75</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>76</v>
@@ -5532,41 +5547,41 @@
         <v>98</v>
       </c>
       <c r="AJ32" t="s" s="2">
-        <v>297</v>
+        <v>75</v>
       </c>
       <c r="AK32" t="s" s="2">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="AL32" t="s" s="2">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="AM32" t="s" s="2">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="AN32" t="s" s="2">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="AO32" t="s" s="2">
-        <v>302</v>
+        <v>295</v>
       </c>
     </row>
-    <row r="33" hidden="true">
+    <row r="33">
       <c r="A33" t="s" s="2">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
-        <v>75</v>
+        <v>297</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" t="s" s="2">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="F33" t="s" s="2">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="G33" t="s" s="2">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="H33" t="s" s="2">
         <v>75</v>
@@ -5575,18 +5590,18 @@
         <v>87</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>305</v>
-      </c>
-      <c r="M33" t="s" s="2">
-        <v>306</v>
-      </c>
-      <c r="N33" s="2"/>
+        <v>299</v>
+      </c>
+      <c r="M33" s="2"/>
+      <c r="N33" t="s" s="2">
+        <v>300</v>
+      </c>
       <c r="O33" t="s" s="2">
         <v>75</v>
       </c>
@@ -5610,13 +5625,11 @@
         <v>75</v>
       </c>
       <c r="W33" t="s" s="2">
-        <v>197</v>
-      </c>
-      <c r="X33" t="s" s="2">
-        <v>307</v>
-      </c>
+        <v>257</v>
+      </c>
+      <c r="X33" s="2"/>
       <c r="Y33" t="s" s="2">
-        <v>308</v>
+        <v>301</v>
       </c>
       <c r="Z33" t="s" s="2">
         <v>75</v>
@@ -5634,13 +5647,13 @@
         <v>75</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AG33" t="s" s="2">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="AH33" t="s" s="2">
         <v>75</v>
@@ -5649,41 +5662,41 @@
         <v>98</v>
       </c>
       <c r="AJ33" t="s" s="2">
-        <v>75</v>
+        <v>302</v>
       </c>
       <c r="AK33" t="s" s="2">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="AL33" t="s" s="2">
-        <v>75</v>
+        <v>304</v>
       </c>
       <c r="AM33" t="s" s="2">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="AN33" t="s" s="2">
-        <v>75</v>
+        <v>306</v>
       </c>
       <c r="AO33" t="s" s="2">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
-        <v>313</v>
+        <v>75</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" t="s" s="2">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="F34" t="s" s="2">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="G34" t="s" s="2">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="H34" t="s" s="2">
         <v>75</v>
@@ -5692,18 +5705,18 @@
         <v>87</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>314</v>
+        <v>253</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>316</v>
-      </c>
-      <c r="M34" s="2"/>
-      <c r="N34" t="s" s="2">
-        <v>317</v>
-      </c>
+        <v>310</v>
+      </c>
+      <c r="M34" t="s" s="2">
+        <v>311</v>
+      </c>
+      <c r="N34" s="2"/>
       <c r="O34" t="s" s="2">
         <v>75</v>
       </c>
@@ -5727,13 +5740,13 @@
         <v>75</v>
       </c>
       <c r="W34" t="s" s="2">
-        <v>75</v>
+        <v>197</v>
       </c>
       <c r="X34" t="s" s="2">
-        <v>75</v>
+        <v>312</v>
       </c>
       <c r="Y34" t="s" s="2">
-        <v>75</v>
+        <v>313</v>
       </c>
       <c r="Z34" t="s" s="2">
         <v>75</v>
@@ -5751,13 +5764,13 @@
         <v>75</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="AF34" t="s" s="2">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="AG34" t="s" s="2">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="AH34" t="s" s="2">
         <v>75</v>
@@ -5766,41 +5779,41 @@
         <v>98</v>
       </c>
       <c r="AJ34" t="s" s="2">
-        <v>318</v>
+        <v>75</v>
       </c>
       <c r="AK34" t="s" s="2">
-        <v>75</v>
+        <v>314</v>
       </c>
       <c r="AL34" t="s" s="2">
-        <v>319</v>
+        <v>75</v>
       </c>
       <c r="AM34" t="s" s="2">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="AN34" t="s" s="2">
-        <v>321</v>
+        <v>75</v>
       </c>
       <c r="AO34" t="s" s="2">
-        <v>75</v>
+        <v>316</v>
       </c>
     </row>
-    <row r="35" hidden="true">
+    <row r="35">
       <c r="A35" t="s" s="2">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
-        <v>75</v>
+        <v>318</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" t="s" s="2">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="F35" t="s" s="2">
         <v>86</v>
       </c>
       <c r="G35" t="s" s="2">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="H35" t="s" s="2">
         <v>75</v>
@@ -5809,18 +5822,18 @@
         <v>87</v>
       </c>
       <c r="J35" t="s" s="2">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>325</v>
-      </c>
-      <c r="M35" t="s" s="2">
-        <v>326</v>
-      </c>
-      <c r="N35" s="2"/>
+        <v>321</v>
+      </c>
+      <c r="M35" s="2"/>
+      <c r="N35" t="s" s="2">
+        <v>322</v>
+      </c>
       <c r="O35" t="s" s="2">
         <v>75</v>
       </c>
@@ -5868,10 +5881,10 @@
         <v>75</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="AF35" t="s" s="2">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="AG35" t="s" s="2">
         <v>86</v>
@@ -5883,19 +5896,19 @@
         <v>98</v>
       </c>
       <c r="AJ35" t="s" s="2">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="AK35" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AL35" t="s" s="2">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="AM35" t="s" s="2">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="AN35" t="s" s="2">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="AO35" t="s" s="2">
         <v>75</v>
@@ -5903,7 +5916,7 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5926,16 +5939,16 @@
         <v>87</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="M36" t="s" s="2">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="N36" s="2"/>
       <c r="O36" t="s" s="2">
@@ -5985,7 +5998,7 @@
         <v>75</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>76</v>
@@ -6000,19 +6013,19 @@
         <v>98</v>
       </c>
       <c r="AJ36" t="s" s="2">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="AK36" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="AM36" t="s" s="2">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="AN36" t="s" s="2">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="AO36" t="s" s="2">
         <v>75</v>
@@ -6020,7 +6033,7 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -6040,19 +6053,19 @@
         <v>75</v>
       </c>
       <c r="I37" t="s" s="2">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>332</v>
+        <v>337</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="M37" t="s" s="2">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="N37" s="2"/>
       <c r="O37" t="s" s="2">
@@ -6102,7 +6115,7 @@
         <v>75</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>76</v>
@@ -6111,33 +6124,33 @@
         <v>86</v>
       </c>
       <c r="AH37" t="s" s="2">
-        <v>344</v>
+        <v>75</v>
       </c>
       <c r="AI37" t="s" s="2">
         <v>98</v>
       </c>
       <c r="AJ37" t="s" s="2">
-        <v>75</v>
+        <v>341</v>
       </c>
       <c r="AK37" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>75</v>
+        <v>342</v>
       </c>
       <c r="AM37" t="s" s="2">
+        <v>343</v>
+      </c>
+      <c r="AN37" t="s" s="2">
+        <v>344</v>
+      </c>
+      <c r="AO37" t="s" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="38" hidden="true">
+      <c r="A38" t="s" s="2">
         <v>345</v>
-      </c>
-      <c r="AN37" t="s" s="2">
-        <v>346</v>
-      </c>
-      <c r="AO37" t="s" s="2">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="s" s="2">
-        <v>347</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -6145,30 +6158,32 @@
       </c>
       <c r="D38" s="2"/>
       <c r="E38" t="s" s="2">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="F38" t="s" s="2">
         <v>86</v>
       </c>
       <c r="G38" t="s" s="2">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="H38" t="s" s="2">
         <v>75</v>
       </c>
       <c r="I38" t="s" s="2">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="J38" t="s" s="2">
+        <v>337</v>
+      </c>
+      <c r="K38" t="s" s="2">
+        <v>346</v>
+      </c>
+      <c r="L38" t="s" s="2">
+        <v>347</v>
+      </c>
+      <c r="M38" t="s" s="2">
         <v>348</v>
       </c>
-      <c r="K38" t="s" s="2">
-        <v>349</v>
-      </c>
-      <c r="L38" t="s" s="2">
-        <v>350</v>
-      </c>
-      <c r="M38" s="2"/>
       <c r="N38" s="2"/>
       <c r="O38" t="s" s="2">
         <v>75</v>
@@ -6217,7 +6232,7 @@
         <v>75</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>76</v>
@@ -6226,7 +6241,7 @@
         <v>86</v>
       </c>
       <c r="AH38" t="s" s="2">
-        <v>75</v>
+        <v>349</v>
       </c>
       <c r="AI38" t="s" s="2">
         <v>98</v>
@@ -6238,21 +6253,21 @@
         <v>75</v>
       </c>
       <c r="AL38" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AM38" t="s" s="2">
+        <v>350</v>
+      </c>
+      <c r="AN38" t="s" s="2">
         <v>351</v>
       </c>
-      <c r="AM38" t="s" s="2">
+      <c r="AO38" t="s" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s" s="2">
         <v>352</v>
-      </c>
-      <c r="AN38" t="s" s="2">
-        <v>353</v>
-      </c>
-      <c r="AO38" t="s" s="2">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="39" hidden="true">
-      <c r="A39" t="s" s="2">
-        <v>354</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -6260,13 +6275,13 @@
       </c>
       <c r="D39" s="2"/>
       <c r="E39" t="s" s="2">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="F39" t="s" s="2">
         <v>86</v>
       </c>
       <c r="G39" t="s" s="2">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="H39" t="s" s="2">
         <v>75</v>
@@ -6275,13 +6290,13 @@
         <v>87</v>
       </c>
       <c r="J39" t="s" s="2">
+        <v>353</v>
+      </c>
+      <c r="K39" t="s" s="2">
+        <v>354</v>
+      </c>
+      <c r="L39" t="s" s="2">
         <v>355</v>
-      </c>
-      <c r="K39" t="s" s="2">
-        <v>356</v>
-      </c>
-      <c r="L39" t="s" s="2">
-        <v>357</v>
       </c>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
@@ -6332,7 +6347,7 @@
         <v>75</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>76</v>
@@ -6353,13 +6368,13 @@
         <v>75</v>
       </c>
       <c r="AL39" t="s" s="2">
-        <v>75</v>
+        <v>356</v>
       </c>
       <c r="AM39" t="s" s="2">
+        <v>357</v>
+      </c>
+      <c r="AN39" t="s" s="2">
         <v>358</v>
-      </c>
-      <c r="AN39" t="s" s="2">
-        <v>359</v>
       </c>
       <c r="AO39" t="s" s="2">
         <v>75</v>
@@ -6367,7 +6382,7 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -6390,7 +6405,7 @@
         <v>87</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>355</v>
+        <v>360</v>
       </c>
       <c r="K40" t="s" s="2">
         <v>361</v>
@@ -6447,7 +6462,7 @@
         <v>75</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>76</v>
@@ -6468,13 +6483,13 @@
         <v>75</v>
       </c>
       <c r="AL40" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AM40" t="s" s="2">
         <v>363</v>
       </c>
-      <c r="AM40" t="s" s="2">
+      <c r="AN40" t="s" s="2">
         <v>364</v>
-      </c>
-      <c r="AN40" t="s" s="2">
-        <v>365</v>
       </c>
       <c r="AO40" t="s" s="2">
         <v>75</v>
@@ -6482,7 +6497,7 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -6493,7 +6508,7 @@
         <v>76</v>
       </c>
       <c r="F41" t="s" s="2">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="G41" t="s" s="2">
         <v>75</v>
@@ -6502,16 +6517,16 @@
         <v>75</v>
       </c>
       <c r="I41" t="s" s="2">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="J41" t="s" s="2">
+        <v>360</v>
+      </c>
+      <c r="K41" t="s" s="2">
+        <v>366</v>
+      </c>
+      <c r="L41" t="s" s="2">
         <v>367</v>
-      </c>
-      <c r="K41" t="s" s="2">
-        <v>368</v>
-      </c>
-      <c r="L41" t="s" s="2">
-        <v>369</v>
       </c>
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
@@ -6562,34 +6577,34 @@
         <v>75</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AG41" t="s" s="2">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="AH41" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AI41" t="s" s="2">
+        <v>98</v>
+      </c>
+      <c r="AJ41" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AK41" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AL41" t="s" s="2">
+        <v>368</v>
+      </c>
+      <c r="AM41" t="s" s="2">
+        <v>369</v>
+      </c>
+      <c r="AN41" t="s" s="2">
         <v>370</v>
-      </c>
-      <c r="AJ41" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AK41" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AL41" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AM41" t="s" s="2">
-        <v>371</v>
-      </c>
-      <c r="AN41" t="s" s="2">
-        <v>75</v>
       </c>
       <c r="AO41" t="s" s="2">
         <v>75</v>
@@ -6597,7 +6612,7 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -6608,7 +6623,7 @@
         <v>76</v>
       </c>
       <c r="F42" t="s" s="2">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="G42" t="s" s="2">
         <v>75</v>
@@ -6620,13 +6635,13 @@
         <v>75</v>
       </c>
       <c r="J42" t="s" s="2">
-        <v>88</v>
+        <v>372</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>100</v>
+        <v>373</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>101</v>
+        <v>374</v>
       </c>
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
@@ -6677,19 +6692,19 @@
         <v>75</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>102</v>
+        <v>371</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AG42" t="s" s="2">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="AH42" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AI42" t="s" s="2">
-        <v>75</v>
+        <v>375</v>
       </c>
       <c r="AJ42" t="s" s="2">
         <v>75</v>
@@ -6701,7 +6716,7 @@
         <v>75</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>103</v>
+        <v>376</v>
       </c>
       <c r="AN42" t="s" s="2">
         <v>75</v>
@@ -6712,18 +6727,18 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>373</v>
+        <v>377</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" t="s" s="2">
         <v>76</v>
       </c>
       <c r="F43" t="s" s="2">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="G43" t="s" s="2">
         <v>75</v>
@@ -6735,17 +6750,15 @@
         <v>75</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>108</v>
-      </c>
-      <c r="M43" t="s" s="2">
-        <v>109</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="M43" s="2"/>
       <c r="N43" s="2"/>
       <c r="O43" t="s" s="2">
         <v>75</v>
@@ -6794,19 +6807,19 @@
         <v>75</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AG43" t="s" s="2">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="AH43" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AI43" t="s" s="2">
-        <v>114</v>
+        <v>75</v>
       </c>
       <c r="AJ43" t="s" s="2">
         <v>75</v>
@@ -6829,11 +6842,11 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>374</v>
+        <v>378</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
-        <v>375</v>
+        <v>105</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" t="s" s="2">
@@ -6846,26 +6859,24 @@
         <v>75</v>
       </c>
       <c r="H44" t="s" s="2">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="I44" t="s" s="2">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="J44" t="s" s="2">
         <v>106</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>376</v>
+        <v>107</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>377</v>
+        <v>108</v>
       </c>
       <c r="M44" t="s" s="2">
         <v>109</v>
       </c>
-      <c r="N44" t="s" s="2">
-        <v>236</v>
-      </c>
+      <c r="N44" s="2"/>
       <c r="O44" t="s" s="2">
         <v>75</v>
       </c>
@@ -6913,7 +6924,7 @@
         <v>75</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>378</v>
+        <v>113</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>76</v>
@@ -6937,7 +6948,7 @@
         <v>75</v>
       </c>
       <c r="AM44" t="s" s="2">
-        <v>229</v>
+        <v>103</v>
       </c>
       <c r="AN44" t="s" s="2">
         <v>75</v>
@@ -6952,35 +6963,39 @@
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
-        <v>75</v>
+        <v>380</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" t="s" s="2">
         <v>76</v>
       </c>
       <c r="F45" t="s" s="2">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="G45" t="s" s="2">
         <v>75</v>
       </c>
       <c r="H45" t="s" s="2">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="I45" t="s" s="2">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="J45" t="s" s="2">
-        <v>248</v>
+        <v>106</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>381</v>
-      </c>
-      <c r="M45" s="2"/>
-      <c r="N45" s="2"/>
+        <v>382</v>
+      </c>
+      <c r="M45" t="s" s="2">
+        <v>109</v>
+      </c>
+      <c r="N45" t="s" s="2">
+        <v>241</v>
+      </c>
       <c r="O45" t="s" s="2">
         <v>75</v>
       </c>
@@ -7004,55 +7019,55 @@
         <v>75</v>
       </c>
       <c r="W45" t="s" s="2">
-        <v>197</v>
+        <v>75</v>
       </c>
       <c r="X45" t="s" s="2">
-        <v>382</v>
+        <v>75</v>
       </c>
       <c r="Y45" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Z45" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AA45" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AB45" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AC45" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AD45" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AE45" t="s" s="2">
         <v>383</v>
       </c>
-      <c r="Z45" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AA45" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AB45" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AC45" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AD45" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AE45" t="s" s="2">
-        <v>379</v>
-      </c>
       <c r="AF45" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AG45" t="s" s="2">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="AH45" t="s" s="2">
-        <v>384</v>
+        <v>75</v>
       </c>
       <c r="AI45" t="s" s="2">
-        <v>98</v>
+        <v>114</v>
       </c>
       <c r="AJ45" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AK45" t="s" s="2">
-        <v>385</v>
+        <v>75</v>
       </c>
       <c r="AL45" t="s" s="2">
-        <v>258</v>
+        <v>75</v>
       </c>
       <c r="AM45" t="s" s="2">
-        <v>300</v>
+        <v>229</v>
       </c>
       <c r="AN45" t="s" s="2">
         <v>75</v>
@@ -7063,7 +7078,7 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -7086,13 +7101,13 @@
         <v>75</v>
       </c>
       <c r="J46" t="s" s="2">
-        <v>88</v>
+        <v>253</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>100</v>
+        <v>385</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>101</v>
+        <v>386</v>
       </c>
       <c r="M46" s="2"/>
       <c r="N46" s="2"/>
@@ -7119,13 +7134,13 @@
         <v>75</v>
       </c>
       <c r="W46" t="s" s="2">
-        <v>75</v>
+        <v>197</v>
       </c>
       <c r="X46" t="s" s="2">
-        <v>75</v>
+        <v>387</v>
       </c>
       <c r="Y46" t="s" s="2">
-        <v>75</v>
+        <v>388</v>
       </c>
       <c r="Z46" t="s" s="2">
         <v>75</v>
@@ -7143,7 +7158,7 @@
         <v>75</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>102</v>
+        <v>384</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>76</v>
@@ -7152,22 +7167,22 @@
         <v>86</v>
       </c>
       <c r="AH46" t="s" s="2">
-        <v>75</v>
+        <v>389</v>
       </c>
       <c r="AI46" t="s" s="2">
-        <v>75</v>
+        <v>98</v>
       </c>
       <c r="AJ46" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AK46" t="s" s="2">
-        <v>75</v>
+        <v>390</v>
       </c>
       <c r="AL46" t="s" s="2">
-        <v>75</v>
+        <v>263</v>
       </c>
       <c r="AM46" t="s" s="2">
-        <v>103</v>
+        <v>305</v>
       </c>
       <c r="AN46" t="s" s="2">
         <v>75</v>
@@ -7178,18 +7193,18 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>387</v>
+        <v>391</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" t="s" s="2">
         <v>76</v>
       </c>
       <c r="F47" t="s" s="2">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="G47" t="s" s="2">
         <v>75</v>
@@ -7201,17 +7216,15 @@
         <v>75</v>
       </c>
       <c r="J47" t="s" s="2">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>108</v>
-      </c>
-      <c r="M47" t="s" s="2">
-        <v>109</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="M47" s="2"/>
       <c r="N47" s="2"/>
       <c r="O47" t="s" s="2">
         <v>75</v>
@@ -7248,31 +7261,31 @@
         <v>75</v>
       </c>
       <c r="AA47" t="s" s="2">
-        <v>110</v>
+        <v>75</v>
       </c>
       <c r="AB47" t="s" s="2">
-        <v>111</v>
+        <v>75</v>
       </c>
       <c r="AC47" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AD47" t="s" s="2">
-        <v>112</v>
+        <v>75</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AG47" t="s" s="2">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="AH47" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AI47" t="s" s="2">
-        <v>114</v>
+        <v>75</v>
       </c>
       <c r="AJ47" t="s" s="2">
         <v>75</v>
@@ -7295,15 +7308,15 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>388</v>
+        <v>392</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
-        <v>75</v>
+        <v>105</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" t="s" s="2">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="F48" t="s" s="2">
         <v>77</v>
@@ -7315,23 +7328,21 @@
         <v>75</v>
       </c>
       <c r="I48" t="s" s="2">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="J48" t="s" s="2">
-        <v>140</v>
+        <v>106</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>389</v>
+        <v>107</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>390</v>
+        <v>108</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>391</v>
-      </c>
-      <c r="N48" t="s" s="2">
-        <v>392</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="N48" s="2"/>
       <c r="O48" t="s" s="2">
         <v>75</v>
       </c>
@@ -7367,10 +7378,10 @@
         <v>75</v>
       </c>
       <c r="AA48" t="s" s="2">
-        <v>147</v>
+        <v>110</v>
       </c>
       <c r="AB48" t="s" s="2">
-        <v>393</v>
+        <v>111</v>
       </c>
       <c r="AC48" t="s" s="2">
         <v>75</v>
@@ -7379,7 +7390,7 @@
         <v>112</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>394</v>
+        <v>113</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>76</v>
@@ -7391,7 +7402,7 @@
         <v>75</v>
       </c>
       <c r="AI48" t="s" s="2">
-        <v>98</v>
+        <v>114</v>
       </c>
       <c r="AJ48" t="s" s="2">
         <v>75</v>
@@ -7400,10 +7411,10 @@
         <v>75</v>
       </c>
       <c r="AL48" t="s" s="2">
-        <v>395</v>
+        <v>75</v>
       </c>
       <c r="AM48" t="s" s="2">
-        <v>396</v>
+        <v>103</v>
       </c>
       <c r="AN48" t="s" s="2">
         <v>75</v>
@@ -7412,13 +7423,11 @@
         <v>75</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>388</v>
-      </c>
-      <c r="B49" t="s" s="2">
-        <v>397</v>
-      </c>
+        <v>393</v>
+      </c>
+      <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
         <v>75</v>
       </c>
@@ -7427,10 +7436,10 @@
         <v>86</v>
       </c>
       <c r="F49" t="s" s="2">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="G49" t="s" s="2">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="H49" t="s" s="2">
         <v>75</v>
@@ -7442,16 +7451,16 @@
         <v>140</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>389</v>
+        <v>394</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>390</v>
+        <v>395</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>391</v>
+        <v>396</v>
       </c>
       <c r="N49" t="s" s="2">
-        <v>392</v>
+        <v>397</v>
       </c>
       <c r="O49" t="s" s="2">
         <v>75</v>
@@ -7488,19 +7497,19 @@
         <v>75</v>
       </c>
       <c r="AA49" t="s" s="2">
-        <v>75</v>
+        <v>147</v>
       </c>
       <c r="AB49" t="s" s="2">
-        <v>75</v>
+        <v>398</v>
       </c>
       <c r="AC49" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AD49" t="s" s="2">
-        <v>75</v>
+        <v>112</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>394</v>
+        <v>399</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>76</v>
@@ -7521,10 +7530,10 @@
         <v>75</v>
       </c>
       <c r="AL49" t="s" s="2">
-        <v>395</v>
+        <v>400</v>
       </c>
       <c r="AM49" t="s" s="2">
-        <v>396</v>
+        <v>401</v>
       </c>
       <c r="AN49" t="s" s="2">
         <v>75</v>
@@ -7533,41 +7542,47 @@
         <v>75</v>
       </c>
     </row>
-    <row r="50" hidden="true">
+    <row r="50">
       <c r="A50" t="s" s="2">
-        <v>398</v>
-      </c>
-      <c r="B50" s="2"/>
+        <v>393</v>
+      </c>
+      <c r="B50" t="s" s="2">
+        <v>402</v>
+      </c>
       <c r="C50" t="s" s="2">
         <v>75</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" t="s" s="2">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="F50" t="s" s="2">
         <v>86</v>
       </c>
       <c r="G50" t="s" s="2">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="H50" t="s" s="2">
         <v>75</v>
       </c>
       <c r="I50" t="s" s="2">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="J50" t="s" s="2">
-        <v>88</v>
+        <v>140</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>100</v>
+        <v>394</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>101</v>
-      </c>
-      <c r="M50" s="2"/>
-      <c r="N50" s="2"/>
+        <v>395</v>
+      </c>
+      <c r="M50" t="s" s="2">
+        <v>396</v>
+      </c>
+      <c r="N50" t="s" s="2">
+        <v>397</v>
+      </c>
       <c r="O50" t="s" s="2">
         <v>75</v>
       </c>
@@ -7615,19 +7630,19 @@
         <v>75</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>102</v>
+        <v>399</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AG50" t="s" s="2">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="AH50" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AI50" t="s" s="2">
-        <v>75</v>
+        <v>98</v>
       </c>
       <c r="AJ50" t="s" s="2">
         <v>75</v>
@@ -7636,10 +7651,10 @@
         <v>75</v>
       </c>
       <c r="AL50" t="s" s="2">
-        <v>75</v>
+        <v>400</v>
       </c>
       <c r="AM50" t="s" s="2">
-        <v>103</v>
+        <v>401</v>
       </c>
       <c r="AN50" t="s" s="2">
         <v>75</v>
@@ -7650,18 +7665,18 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>399</v>
+        <v>403</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" t="s" s="2">
         <v>76</v>
       </c>
       <c r="F51" t="s" s="2">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="G51" t="s" s="2">
         <v>75</v>
@@ -7673,17 +7688,15 @@
         <v>75</v>
       </c>
       <c r="J51" t="s" s="2">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>108</v>
-      </c>
-      <c r="M51" t="s" s="2">
-        <v>109</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="M51" s="2"/>
       <c r="N51" s="2"/>
       <c r="O51" t="s" s="2">
         <v>75</v>
@@ -7720,31 +7733,31 @@
         <v>75</v>
       </c>
       <c r="AA51" t="s" s="2">
-        <v>110</v>
+        <v>75</v>
       </c>
       <c r="AB51" t="s" s="2">
-        <v>111</v>
+        <v>75</v>
       </c>
       <c r="AC51" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AD51" t="s" s="2">
-        <v>112</v>
+        <v>75</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AG51" t="s" s="2">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="AH51" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AI51" t="s" s="2">
-        <v>114</v>
+        <v>75</v>
       </c>
       <c r="AJ51" t="s" s="2">
         <v>75</v>
@@ -7767,18 +7780,18 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>400</v>
+        <v>404</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
-        <v>75</v>
+        <v>105</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" t="s" s="2">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="F52" t="s" s="2">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="G52" t="s" s="2">
         <v>75</v>
@@ -7787,23 +7800,21 @@
         <v>75</v>
       </c>
       <c r="I52" t="s" s="2">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="J52" t="s" s="2">
-        <v>128</v>
+        <v>106</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>154</v>
+        <v>107</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>155</v>
+        <v>108</v>
       </c>
       <c r="M52" t="s" s="2">
-        <v>156</v>
-      </c>
-      <c r="N52" t="s" s="2">
-        <v>157</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="N52" s="2"/>
       <c r="O52" t="s" s="2">
         <v>75</v>
       </c>
@@ -7812,7 +7823,7 @@
         <v>75</v>
       </c>
       <c r="R52" t="s" s="2">
-        <v>401</v>
+        <v>75</v>
       </c>
       <c r="S52" t="s" s="2">
         <v>75</v>
@@ -7839,31 +7850,31 @@
         <v>75</v>
       </c>
       <c r="AA52" t="s" s="2">
-        <v>75</v>
+        <v>110</v>
       </c>
       <c r="AB52" t="s" s="2">
-        <v>75</v>
+        <v>111</v>
       </c>
       <c r="AC52" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AD52" t="s" s="2">
-        <v>75</v>
+        <v>112</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>159</v>
+        <v>113</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AG52" t="s" s="2">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="AH52" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AI52" t="s" s="2">
-        <v>98</v>
+        <v>114</v>
       </c>
       <c r="AJ52" t="s" s="2">
         <v>75</v>
@@ -7872,10 +7883,10 @@
         <v>75</v>
       </c>
       <c r="AL52" t="s" s="2">
-        <v>160</v>
+        <v>75</v>
       </c>
       <c r="AM52" t="s" s="2">
-        <v>161</v>
+        <v>103</v>
       </c>
       <c r="AN52" t="s" s="2">
         <v>75</v>
@@ -7886,7 +7897,7 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>402</v>
+        <v>405</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
@@ -7894,7 +7905,7 @@
       </c>
       <c r="D53" s="2"/>
       <c r="E53" t="s" s="2">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="F53" t="s" s="2">
         <v>86</v>
@@ -7909,18 +7920,20 @@
         <v>87</v>
       </c>
       <c r="J53" t="s" s="2">
-        <v>88</v>
+        <v>128</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="M53" t="s" s="2">
-        <v>165</v>
-      </c>
-      <c r="N53" s="2"/>
+        <v>156</v>
+      </c>
+      <c r="N53" t="s" s="2">
+        <v>157</v>
+      </c>
       <c r="O53" t="s" s="2">
         <v>75</v>
       </c>
@@ -7929,7 +7942,7 @@
         <v>75</v>
       </c>
       <c r="R53" t="s" s="2">
-        <v>75</v>
+        <v>406</v>
       </c>
       <c r="S53" t="s" s="2">
         <v>75</v>
@@ -7968,7 +7981,7 @@
         <v>75</v>
       </c>
       <c r="AE53" t="s" s="2">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="AF53" t="s" s="2">
         <v>76</v>
@@ -7989,10 +8002,10 @@
         <v>75</v>
       </c>
       <c r="AL53" t="s" s="2">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="AM53" t="s" s="2">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="AN53" t="s" s="2">
         <v>75</v>
@@ -8003,7 +8016,7 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>403</v>
+        <v>407</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
@@ -8011,7 +8024,7 @@
       </c>
       <c r="D54" s="2"/>
       <c r="E54" t="s" s="2">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="F54" t="s" s="2">
         <v>86</v>
@@ -8026,18 +8039,18 @@
         <v>87</v>
       </c>
       <c r="J54" t="s" s="2">
-        <v>170</v>
+        <v>88</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>172</v>
-      </c>
-      <c r="M54" s="2"/>
-      <c r="N54" t="s" s="2">
-        <v>173</v>
-      </c>
+        <v>164</v>
+      </c>
+      <c r="M54" t="s" s="2">
+        <v>165</v>
+      </c>
+      <c r="N54" s="2"/>
       <c r="O54" t="s" s="2">
         <v>75</v>
       </c>
@@ -8061,11 +8074,13 @@
         <v>75</v>
       </c>
       <c r="W54" t="s" s="2">
-        <v>252</v>
-      </c>
-      <c r="X54" s="2"/>
+        <v>75</v>
+      </c>
+      <c r="X54" t="s" s="2">
+        <v>75</v>
+      </c>
       <c r="Y54" t="s" s="2">
-        <v>404</v>
+        <v>75</v>
       </c>
       <c r="Z54" t="s" s="2">
         <v>75</v>
@@ -8083,7 +8098,7 @@
         <v>75</v>
       </c>
       <c r="AE54" t="s" s="2">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="AF54" t="s" s="2">
         <v>76</v>
@@ -8104,10 +8119,10 @@
         <v>75</v>
       </c>
       <c r="AL54" t="s" s="2">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="AM54" t="s" s="2">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="AN54" t="s" s="2">
         <v>75</v>
@@ -8118,7 +8133,7 @@
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" t="s" s="2">
@@ -8126,7 +8141,7 @@
       </c>
       <c r="D55" s="2"/>
       <c r="E55" t="s" s="2">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="F55" t="s" s="2">
         <v>86</v>
@@ -8141,17 +8156,17 @@
         <v>87</v>
       </c>
       <c r="J55" t="s" s="2">
-        <v>88</v>
+        <v>170</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="M55" s="2"/>
       <c r="N55" t="s" s="2">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="O55" t="s" s="2">
         <v>75</v>
@@ -8176,13 +8191,11 @@
         <v>75</v>
       </c>
       <c r="W55" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="X55" t="s" s="2">
-        <v>75</v>
-      </c>
+        <v>257</v>
+      </c>
+      <c r="X55" s="2"/>
       <c r="Y55" t="s" s="2">
-        <v>75</v>
+        <v>409</v>
       </c>
       <c r="Z55" t="s" s="2">
         <v>75</v>
@@ -8200,7 +8213,7 @@
         <v>75</v>
       </c>
       <c r="AE55" t="s" s="2">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="AF55" t="s" s="2">
         <v>76</v>
@@ -8221,10 +8234,10 @@
         <v>75</v>
       </c>
       <c r="AL55" t="s" s="2">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="AM55" t="s" s="2">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="AN55" t="s" s="2">
         <v>75</v>
@@ -8235,7 +8248,7 @@
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>406</v>
+        <v>410</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
@@ -8258,19 +8271,17 @@
         <v>87</v>
       </c>
       <c r="J56" t="s" s="2">
-        <v>185</v>
+        <v>88</v>
       </c>
       <c r="K56" t="s" s="2">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>187</v>
-      </c>
-      <c r="M56" t="s" s="2">
-        <v>188</v>
-      </c>
+        <v>179</v>
+      </c>
+      <c r="M56" s="2"/>
       <c r="N56" t="s" s="2">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="O56" t="s" s="2">
         <v>75</v>
@@ -8319,7 +8330,7 @@
         <v>75</v>
       </c>
       <c r="AE56" t="s" s="2">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="AF56" t="s" s="2">
         <v>76</v>
@@ -8340,10 +8351,10 @@
         <v>75</v>
       </c>
       <c r="AL56" t="s" s="2">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="AM56" t="s" s="2">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="AN56" t="s" s="2">
         <v>75</v>
@@ -8354,7 +8365,7 @@
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>407</v>
+        <v>411</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
@@ -8377,19 +8388,19 @@
         <v>87</v>
       </c>
       <c r="J57" t="s" s="2">
-        <v>88</v>
+        <v>185</v>
       </c>
       <c r="K57" t="s" s="2">
-        <v>408</v>
+        <v>186</v>
       </c>
       <c r="L57" t="s" s="2">
-        <v>409</v>
+        <v>187</v>
       </c>
       <c r="M57" t="s" s="2">
-        <v>410</v>
+        <v>188</v>
       </c>
       <c r="N57" t="s" s="2">
-        <v>411</v>
+        <v>189</v>
       </c>
       <c r="O57" t="s" s="2">
         <v>75</v>
@@ -8438,7 +8449,7 @@
         <v>75</v>
       </c>
       <c r="AE57" t="s" s="2">
-        <v>412</v>
+        <v>190</v>
       </c>
       <c r="AF57" t="s" s="2">
         <v>76</v>
@@ -8459,10 +8470,10 @@
         <v>75</v>
       </c>
       <c r="AL57" t="s" s="2">
-        <v>413</v>
+        <v>191</v>
       </c>
       <c r="AM57" t="s" s="2">
-        <v>414</v>
+        <v>192</v>
       </c>
       <c r="AN57" t="s" s="2">
         <v>75</v>
@@ -8473,7 +8484,7 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
@@ -8484,7 +8495,7 @@
         <v>76</v>
       </c>
       <c r="F58" t="s" s="2">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="G58" t="s" s="2">
         <v>75</v>
@@ -8493,19 +8504,23 @@
         <v>75</v>
       </c>
       <c r="I58" t="s" s="2">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="J58" t="s" s="2">
+        <v>88</v>
+      </c>
+      <c r="K58" t="s" s="2">
+        <v>413</v>
+      </c>
+      <c r="L58" t="s" s="2">
+        <v>414</v>
+      </c>
+      <c r="M58" t="s" s="2">
+        <v>415</v>
+      </c>
+      <c r="N58" t="s" s="2">
         <v>416</v>
       </c>
-      <c r="K58" t="s" s="2">
-        <v>417</v>
-      </c>
-      <c r="L58" t="s" s="2">
-        <v>418</v>
-      </c>
-      <c r="M58" s="2"/>
-      <c r="N58" s="2"/>
       <c r="O58" t="s" s="2">
         <v>75</v>
       </c>
@@ -8553,16 +8568,16 @@
         <v>75</v>
       </c>
       <c r="AE58" t="s" s="2">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="AF58" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AG58" t="s" s="2">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="AH58" t="s" s="2">
-        <v>384</v>
+        <v>75</v>
       </c>
       <c r="AI58" t="s" s="2">
         <v>98</v>
@@ -8574,7 +8589,7 @@
         <v>75</v>
       </c>
       <c r="AL58" t="s" s="2">
-        <v>75</v>
+        <v>418</v>
       </c>
       <c r="AM58" t="s" s="2">
         <v>419</v>
@@ -8599,7 +8614,7 @@
         <v>76</v>
       </c>
       <c r="F59" t="s" s="2">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="G59" t="s" s="2">
         <v>75</v>
@@ -8611,13 +8626,13 @@
         <v>75</v>
       </c>
       <c r="J59" t="s" s="2">
-        <v>248</v>
+        <v>421</v>
       </c>
       <c r="K59" t="s" s="2">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="M59" s="2"/>
       <c r="N59" s="2"/>
@@ -8644,13 +8659,13 @@
         <v>75</v>
       </c>
       <c r="W59" t="s" s="2">
-        <v>197</v>
+        <v>75</v>
       </c>
       <c r="X59" t="s" s="2">
-        <v>423</v>
+        <v>75</v>
       </c>
       <c r="Y59" t="s" s="2">
-        <v>424</v>
+        <v>75</v>
       </c>
       <c r="Z59" t="s" s="2">
         <v>75</v>
@@ -8674,10 +8689,10 @@
         <v>76</v>
       </c>
       <c r="AG59" t="s" s="2">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="AH59" t="s" s="2">
-        <v>75</v>
+        <v>389</v>
       </c>
       <c r="AI59" t="s" s="2">
         <v>98</v>
@@ -8692,7 +8707,7 @@
         <v>75</v>
       </c>
       <c r="AM59" t="s" s="2">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="AN59" t="s" s="2">
         <v>75</v>
@@ -8703,7 +8718,7 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
@@ -8714,7 +8729,7 @@
         <v>76</v>
       </c>
       <c r="F60" t="s" s="2">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="G60" t="s" s="2">
         <v>75</v>
@@ -8726,17 +8741,15 @@
         <v>75</v>
       </c>
       <c r="J60" t="s" s="2">
-        <v>367</v>
+        <v>253</v>
       </c>
       <c r="K60" t="s" s="2">
+        <v>426</v>
+      </c>
+      <c r="L60" t="s" s="2">
         <v>427</v>
       </c>
-      <c r="L60" t="s" s="2">
-        <v>428</v>
-      </c>
-      <c r="M60" t="s" s="2">
-        <v>429</v>
-      </c>
+      <c r="M60" s="2"/>
       <c r="N60" s="2"/>
       <c r="O60" t="s" s="2">
         <v>75</v>
@@ -8761,13 +8774,13 @@
         <v>75</v>
       </c>
       <c r="W60" t="s" s="2">
-        <v>75</v>
+        <v>197</v>
       </c>
       <c r="X60" t="s" s="2">
-        <v>75</v>
+        <v>428</v>
       </c>
       <c r="Y60" t="s" s="2">
-        <v>75</v>
+        <v>429</v>
       </c>
       <c r="Z60" t="s" s="2">
         <v>75</v>
@@ -8785,31 +8798,31 @@
         <v>75</v>
       </c>
       <c r="AE60" t="s" s="2">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="AF60" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AG60" t="s" s="2">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="AH60" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AI60" t="s" s="2">
+        <v>98</v>
+      </c>
+      <c r="AJ60" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AK60" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AL60" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AM60" t="s" s="2">
         <v>430</v>
-      </c>
-      <c r="AJ60" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AK60" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AL60" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AM60" t="s" s="2">
-        <v>431</v>
       </c>
       <c r="AN60" t="s" s="2">
         <v>75</v>
@@ -8820,7 +8833,7 @@
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
@@ -8831,7 +8844,7 @@
         <v>76</v>
       </c>
       <c r="F61" t="s" s="2">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="G61" t="s" s="2">
         <v>75</v>
@@ -8843,15 +8856,17 @@
         <v>75</v>
       </c>
       <c r="J61" t="s" s="2">
-        <v>88</v>
+        <v>372</v>
       </c>
       <c r="K61" t="s" s="2">
-        <v>100</v>
+        <v>432</v>
       </c>
       <c r="L61" t="s" s="2">
-        <v>101</v>
-      </c>
-      <c r="M61" s="2"/>
+        <v>433</v>
+      </c>
+      <c r="M61" t="s" s="2">
+        <v>434</v>
+      </c>
       <c r="N61" s="2"/>
       <c r="O61" t="s" s="2">
         <v>75</v>
@@ -8900,19 +8915,19 @@
         <v>75</v>
       </c>
       <c r="AE61" t="s" s="2">
-        <v>102</v>
+        <v>431</v>
       </c>
       <c r="AF61" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AG61" t="s" s="2">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="AH61" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AI61" t="s" s="2">
-        <v>75</v>
+        <v>435</v>
       </c>
       <c r="AJ61" t="s" s="2">
         <v>75</v>
@@ -8924,7 +8939,7 @@
         <v>75</v>
       </c>
       <c r="AM61" t="s" s="2">
-        <v>103</v>
+        <v>436</v>
       </c>
       <c r="AN61" t="s" s="2">
         <v>75</v>
@@ -8935,18 +8950,18 @@
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>433</v>
+        <v>437</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="D62" s="2"/>
       <c r="E62" t="s" s="2">
         <v>76</v>
       </c>
       <c r="F62" t="s" s="2">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="G62" t="s" s="2">
         <v>75</v>
@@ -8958,17 +8973,15 @@
         <v>75</v>
       </c>
       <c r="J62" t="s" s="2">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="K62" t="s" s="2">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="L62" t="s" s="2">
-        <v>108</v>
-      </c>
-      <c r="M62" t="s" s="2">
-        <v>109</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="M62" s="2"/>
       <c r="N62" s="2"/>
       <c r="O62" t="s" s="2">
         <v>75</v>
@@ -9017,19 +9030,19 @@
         <v>75</v>
       </c>
       <c r="AE62" t="s" s="2">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="AF62" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AG62" t="s" s="2">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="AH62" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AI62" t="s" s="2">
-        <v>114</v>
+        <v>75</v>
       </c>
       <c r="AJ62" t="s" s="2">
         <v>75</v>
@@ -9052,11 +9065,11 @@
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>434</v>
+        <v>438</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" t="s" s="2">
-        <v>375</v>
+        <v>105</v>
       </c>
       <c r="D63" s="2"/>
       <c r="E63" t="s" s="2">
@@ -9069,26 +9082,24 @@
         <v>75</v>
       </c>
       <c r="H63" t="s" s="2">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="I63" t="s" s="2">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="J63" t="s" s="2">
         <v>106</v>
       </c>
       <c r="K63" t="s" s="2">
-        <v>376</v>
+        <v>107</v>
       </c>
       <c r="L63" t="s" s="2">
-        <v>377</v>
+        <v>108</v>
       </c>
       <c r="M63" t="s" s="2">
         <v>109</v>
       </c>
-      <c r="N63" t="s" s="2">
-        <v>236</v>
-      </c>
+      <c r="N63" s="2"/>
       <c r="O63" t="s" s="2">
         <v>75</v>
       </c>
@@ -9136,7 +9147,7 @@
         <v>75</v>
       </c>
       <c r="AE63" t="s" s="2">
-        <v>378</v>
+        <v>113</v>
       </c>
       <c r="AF63" t="s" s="2">
         <v>76</v>
@@ -9160,7 +9171,7 @@
         <v>75</v>
       </c>
       <c r="AM63" t="s" s="2">
-        <v>229</v>
+        <v>103</v>
       </c>
       <c r="AN63" t="s" s="2">
         <v>75</v>
@@ -9171,11 +9182,11 @@
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>435</v>
+        <v>439</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" t="s" s="2">
-        <v>75</v>
+        <v>380</v>
       </c>
       <c r="D64" s="2"/>
       <c r="E64" t="s" s="2">
@@ -9188,22 +9199,26 @@
         <v>75</v>
       </c>
       <c r="H64" t="s" s="2">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="I64" t="s" s="2">
         <v>87</v>
       </c>
       <c r="J64" t="s" s="2">
-        <v>248</v>
+        <v>106</v>
       </c>
       <c r="K64" t="s" s="2">
-        <v>436</v>
+        <v>381</v>
       </c>
       <c r="L64" t="s" s="2">
-        <v>437</v>
-      </c>
-      <c r="M64" s="2"/>
-      <c r="N64" s="2"/>
+        <v>382</v>
+      </c>
+      <c r="M64" t="s" s="2">
+        <v>109</v>
+      </c>
+      <c r="N64" t="s" s="2">
+        <v>241</v>
+      </c>
       <c r="O64" t="s" s="2">
         <v>75</v>
       </c>
@@ -9227,13 +9242,13 @@
         <v>75</v>
       </c>
       <c r="W64" t="s" s="2">
-        <v>197</v>
+        <v>75</v>
       </c>
       <c r="X64" t="s" s="2">
-        <v>438</v>
+        <v>75</v>
       </c>
       <c r="Y64" t="s" s="2">
-        <v>439</v>
+        <v>75</v>
       </c>
       <c r="Z64" t="s" s="2">
         <v>75</v>
@@ -9251,7 +9266,7 @@
         <v>75</v>
       </c>
       <c r="AE64" t="s" s="2">
-        <v>435</v>
+        <v>383</v>
       </c>
       <c r="AF64" t="s" s="2">
         <v>76</v>
@@ -9260,25 +9275,25 @@
         <v>77</v>
       </c>
       <c r="AH64" t="s" s="2">
-        <v>440</v>
+        <v>75</v>
       </c>
       <c r="AI64" t="s" s="2">
-        <v>98</v>
+        <v>114</v>
       </c>
       <c r="AJ64" t="s" s="2">
-        <v>441</v>
+        <v>75</v>
       </c>
       <c r="AK64" t="s" s="2">
-        <v>277</v>
+        <v>75</v>
       </c>
       <c r="AL64" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AM64" t="s" s="2">
-        <v>442</v>
+        <v>229</v>
       </c>
       <c r="AN64" t="s" s="2">
-        <v>443</v>
+        <v>75</v>
       </c>
       <c r="AO64" t="s" s="2">
         <v>75</v>
@@ -9286,7 +9301,7 @@
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" t="s" s="2">
@@ -9309,13 +9324,13 @@
         <v>87</v>
       </c>
       <c r="J65" t="s" s="2">
-        <v>445</v>
+        <v>253</v>
       </c>
       <c r="K65" t="s" s="2">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="L65" t="s" s="2">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="M65" s="2"/>
       <c r="N65" s="2"/>
@@ -9342,13 +9357,13 @@
         <v>75</v>
       </c>
       <c r="W65" t="s" s="2">
-        <v>75</v>
+        <v>197</v>
       </c>
       <c r="X65" t="s" s="2">
-        <v>75</v>
+        <v>443</v>
       </c>
       <c r="Y65" t="s" s="2">
-        <v>75</v>
+        <v>444</v>
       </c>
       <c r="Z65" t="s" s="2">
         <v>75</v>
@@ -9366,7 +9381,7 @@
         <v>75</v>
       </c>
       <c r="AE65" t="s" s="2">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="AF65" t="s" s="2">
         <v>76</v>
@@ -9375,25 +9390,25 @@
         <v>77</v>
       </c>
       <c r="AH65" t="s" s="2">
-        <v>440</v>
+        <v>445</v>
       </c>
       <c r="AI65" t="s" s="2">
         <v>98</v>
       </c>
       <c r="AJ65" t="s" s="2">
-        <v>75</v>
+        <v>446</v>
       </c>
       <c r="AK65" t="s" s="2">
-        <v>75</v>
+        <v>282</v>
       </c>
       <c r="AL65" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AM65" t="s" s="2">
-        <v>419</v>
+        <v>447</v>
       </c>
       <c r="AN65" t="s" s="2">
-        <v>443</v>
+        <v>448</v>
       </c>
       <c r="AO65" t="s" s="2">
         <v>75</v>
@@ -9401,7 +9416,7 @@
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" t="s" s="2">
@@ -9421,16 +9436,16 @@
         <v>75</v>
       </c>
       <c r="I66" t="s" s="2">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="J66" t="s" s="2">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="K66" t="s" s="2">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="L66" t="s" s="2">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="M66" s="2"/>
       <c r="N66" s="2"/>
@@ -9481,7 +9496,7 @@
         <v>75</v>
       </c>
       <c r="AE66" t="s" s="2">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="AF66" t="s" s="2">
         <v>76</v>
@@ -9490,32 +9505,147 @@
         <v>77</v>
       </c>
       <c r="AH66" t="s" s="2">
-        <v>75</v>
+        <v>445</v>
       </c>
       <c r="AI66" t="s" s="2">
         <v>98</v>
       </c>
       <c r="AJ66" t="s" s="2">
-        <v>452</v>
+        <v>75</v>
       </c>
       <c r="AK66" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AL66" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AM66" t="s" s="2">
+        <v>424</v>
+      </c>
+      <c r="AN66" t="s" s="2">
+        <v>448</v>
+      </c>
+      <c r="AO66" t="s" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="67" hidden="true">
+      <c r="A67" t="s" s="2">
         <v>453</v>
       </c>
-      <c r="AM66" t="s" s="2">
+      <c r="B67" s="2"/>
+      <c r="C67" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="D67" s="2"/>
+      <c r="E67" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="F67" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="G67" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="H67" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="I67" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="J67" t="s" s="2">
         <v>454</v>
       </c>
-      <c r="AN66" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AO66" t="s" s="2">
+      <c r="K67" t="s" s="2">
+        <v>455</v>
+      </c>
+      <c r="L67" t="s" s="2">
+        <v>456</v>
+      </c>
+      <c r="M67" s="2"/>
+      <c r="N67" s="2"/>
+      <c r="O67" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="P67" s="2"/>
+      <c r="Q67" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="R67" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="S67" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="T67" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="U67" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="V67" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="W67" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="X67" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Y67" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Z67" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AA67" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AB67" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AC67" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AD67" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AE67" t="s" s="2">
+        <v>453</v>
+      </c>
+      <c r="AF67" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AG67" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AH67" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AI67" t="s" s="2">
+        <v>98</v>
+      </c>
+      <c r="AJ67" t="s" s="2">
+        <v>457</v>
+      </c>
+      <c r="AK67" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AL67" t="s" s="2">
+        <v>458</v>
+      </c>
+      <c r="AM67" t="s" s="2">
+        <v>459</v>
+      </c>
+      <c r="AN67" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AO67" t="s" s="2">
         <v>75</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AO66">
+  <autoFilter ref="A1:AO67">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -9525,7 +9655,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI65">
+  <conditionalFormatting sqref="A2:AI66">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>